<commit_message>
Kirk added code to deal with the effect of small groups on joint confidence intervals.
</commit_message>
<xml_diff>
--- a/inst/data_files/SH11SIMPOP_StockSex.xlsx
+++ b/inst/data_files/SH11SIMPOP_StockSex.xlsx
@@ -535,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF28"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -552,11 +552,10 @@
     <col min="7" max="7" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="28" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="58" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="59" max="16384" width="9.140625" style="2"/>
+    <col min="29" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -641,38 +640,8 @@
       <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
-      <c r="AN1" s="1"/>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1"/>
-      <c r="AQ1" s="1"/>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1"/>
-      <c r="AT1" s="1"/>
-      <c r="AU1" s="1"/>
-      <c r="AV1" s="1"/>
-      <c r="AW1" s="1"/>
-      <c r="AX1" s="1"/>
-      <c r="AY1" s="1"/>
-      <c r="AZ1" s="1"/>
-      <c r="BA1" s="1"/>
-      <c r="BB1" s="1"/>
-      <c r="BC1" s="1"/>
-      <c r="BD1" s="1"/>
-      <c r="BE1" s="1"/>
-      <c r="BF1" s="1"/>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -757,38 +726,8 @@
       <c r="AB2" s="8">
         <v>4.5499999999999999E-2</v>
       </c>
-      <c r="AC2" s="8"/>
-      <c r="AD2" s="8"/>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="8"/>
-      <c r="AG2" s="8"/>
-      <c r="AH2" s="8"/>
-      <c r="AI2" s="8"/>
-      <c r="AJ2" s="8"/>
-      <c r="AK2" s="8"/>
-      <c r="AL2" s="8"/>
-      <c r="AM2" s="8"/>
-      <c r="AN2" s="8"/>
-      <c r="AO2" s="8"/>
-      <c r="AP2" s="8"/>
-      <c r="AQ2" s="8"/>
-      <c r="AR2" s="8"/>
-      <c r="AS2" s="8"/>
-      <c r="AT2" s="8"/>
-      <c r="AU2" s="8"/>
-      <c r="AV2" s="8"/>
-      <c r="AW2" s="8"/>
-      <c r="AX2" s="8"/>
-      <c r="AY2" s="8"/>
-      <c r="AZ2" s="8"/>
-      <c r="BA2" s="8"/>
-      <c r="BB2" s="8"/>
-      <c r="BC2" s="8"/>
-      <c r="BD2" s="8"/>
-      <c r="BE2" s="8"/>
-      <c r="BF2" s="8"/>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -873,38 +812,8 @@
       <c r="AB3" s="8">
         <v>0</v>
       </c>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="8"/>
-      <c r="AG3" s="8"/>
-      <c r="AH3" s="8"/>
-      <c r="AI3" s="8"/>
-      <c r="AJ3" s="8"/>
-      <c r="AK3" s="8"/>
-      <c r="AL3" s="8"/>
-      <c r="AM3" s="8"/>
-      <c r="AN3" s="8"/>
-      <c r="AO3" s="8"/>
-      <c r="AP3" s="8"/>
-      <c r="AQ3" s="8"/>
-      <c r="AR3" s="8"/>
-      <c r="AS3" s="8"/>
-      <c r="AT3" s="8"/>
-      <c r="AU3" s="8"/>
-      <c r="AV3" s="8"/>
-      <c r="AW3" s="8"/>
-      <c r="AX3" s="8"/>
-      <c r="AY3" s="8"/>
-      <c r="AZ3" s="8"/>
-      <c r="BA3" s="8"/>
-      <c r="BB3" s="8"/>
-      <c r="BC3" s="8"/>
-      <c r="BD3" s="8"/>
-      <c r="BE3" s="8"/>
-      <c r="BF3" s="8"/>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -989,38 +898,8 @@
       <c r="AB4" s="8">
         <v>4.3499999999999997E-2</v>
       </c>
-      <c r="AC4" s="8"/>
-      <c r="AD4" s="8"/>
-      <c r="AE4" s="8"/>
-      <c r="AF4" s="8"/>
-      <c r="AG4" s="8"/>
-      <c r="AH4" s="8"/>
-      <c r="AI4" s="8"/>
-      <c r="AJ4" s="8"/>
-      <c r="AK4" s="8"/>
-      <c r="AL4" s="8"/>
-      <c r="AM4" s="8"/>
-      <c r="AN4" s="8"/>
-      <c r="AO4" s="8"/>
-      <c r="AP4" s="8"/>
-      <c r="AQ4" s="8"/>
-      <c r="AR4" s="8"/>
-      <c r="AS4" s="8"/>
-      <c r="AT4" s="8"/>
-      <c r="AU4" s="8"/>
-      <c r="AV4" s="8"/>
-      <c r="AW4" s="8"/>
-      <c r="AX4" s="8"/>
-      <c r="AY4" s="8"/>
-      <c r="AZ4" s="8"/>
-      <c r="BA4" s="8"/>
-      <c r="BB4" s="8"/>
-      <c r="BC4" s="8"/>
-      <c r="BD4" s="8"/>
-      <c r="BE4" s="8"/>
-      <c r="BF4" s="8"/>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1105,38 +984,8 @@
       <c r="AB5" s="8">
         <v>4.7600000000000003E-2</v>
       </c>
-      <c r="AC5" s="8"/>
-      <c r="AD5" s="8"/>
-      <c r="AE5" s="8"/>
-      <c r="AF5" s="8"/>
-      <c r="AG5" s="8"/>
-      <c r="AH5" s="8"/>
-      <c r="AI5" s="8"/>
-      <c r="AJ5" s="8"/>
-      <c r="AK5" s="8"/>
-      <c r="AL5" s="8"/>
-      <c r="AM5" s="8"/>
-      <c r="AN5" s="8"/>
-      <c r="AO5" s="8"/>
-      <c r="AP5" s="8"/>
-      <c r="AQ5" s="8"/>
-      <c r="AR5" s="8"/>
-      <c r="AS5" s="8"/>
-      <c r="AT5" s="8"/>
-      <c r="AU5" s="8"/>
-      <c r="AV5" s="8"/>
-      <c r="AW5" s="8"/>
-      <c r="AX5" s="8"/>
-      <c r="AY5" s="8"/>
-      <c r="AZ5" s="8"/>
-      <c r="BA5" s="8"/>
-      <c r="BB5" s="8"/>
-      <c r="BC5" s="8"/>
-      <c r="BD5" s="8"/>
-      <c r="BE5" s="8"/>
-      <c r="BF5" s="8"/>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1221,38 +1070,8 @@
       <c r="AB6" s="8">
         <v>0.13789999999999999</v>
       </c>
-      <c r="AC6" s="8"/>
-      <c r="AD6" s="8"/>
-      <c r="AE6" s="8"/>
-      <c r="AF6" s="8"/>
-      <c r="AG6" s="8"/>
-      <c r="AH6" s="8"/>
-      <c r="AI6" s="8"/>
-      <c r="AJ6" s="8"/>
-      <c r="AK6" s="8"/>
-      <c r="AL6" s="8"/>
-      <c r="AM6" s="8"/>
-      <c r="AN6" s="8"/>
-      <c r="AO6" s="8"/>
-      <c r="AP6" s="8"/>
-      <c r="AQ6" s="8"/>
-      <c r="AR6" s="8"/>
-      <c r="AS6" s="8"/>
-      <c r="AT6" s="8"/>
-      <c r="AU6" s="8"/>
-      <c r="AV6" s="8"/>
-      <c r="AW6" s="8"/>
-      <c r="AX6" s="8"/>
-      <c r="AY6" s="8"/>
-      <c r="AZ6" s="8"/>
-      <c r="BA6" s="8"/>
-      <c r="BB6" s="8"/>
-      <c r="BC6" s="8"/>
-      <c r="BD6" s="8"/>
-      <c r="BE6" s="8"/>
-      <c r="BF6" s="8"/>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1337,38 +1156,8 @@
       <c r="AB7" s="8">
         <v>0.08</v>
       </c>
-      <c r="AC7" s="8"/>
-      <c r="AD7" s="8"/>
-      <c r="AE7" s="8"/>
-      <c r="AF7" s="8"/>
-      <c r="AG7" s="8"/>
-      <c r="AH7" s="8"/>
-      <c r="AI7" s="8"/>
-      <c r="AJ7" s="8"/>
-      <c r="AK7" s="8"/>
-      <c r="AL7" s="8"/>
-      <c r="AM7" s="8"/>
-      <c r="AN7" s="8"/>
-      <c r="AO7" s="8"/>
-      <c r="AP7" s="8"/>
-      <c r="AQ7" s="8"/>
-      <c r="AR7" s="8"/>
-      <c r="AS7" s="8"/>
-      <c r="AT7" s="8"/>
-      <c r="AU7" s="8"/>
-      <c r="AV7" s="8"/>
-      <c r="AW7" s="8"/>
-      <c r="AX7" s="8"/>
-      <c r="AY7" s="8"/>
-      <c r="AZ7" s="8"/>
-      <c r="BA7" s="8"/>
-      <c r="BB7" s="8"/>
-      <c r="BC7" s="8"/>
-      <c r="BD7" s="8"/>
-      <c r="BE7" s="8"/>
-      <c r="BF7" s="8"/>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1453,38 +1242,8 @@
       <c r="AB8" s="8">
         <v>0.1</v>
       </c>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="8"/>
-      <c r="AH8" s="8"/>
-      <c r="AI8" s="8"/>
-      <c r="AJ8" s="8"/>
-      <c r="AK8" s="8"/>
-      <c r="AL8" s="8"/>
-      <c r="AM8" s="8"/>
-      <c r="AN8" s="8"/>
-      <c r="AO8" s="8"/>
-      <c r="AP8" s="8"/>
-      <c r="AQ8" s="8"/>
-      <c r="AR8" s="8"/>
-      <c r="AS8" s="8"/>
-      <c r="AT8" s="8"/>
-      <c r="AU8" s="8"/>
-      <c r="AV8" s="8"/>
-      <c r="AW8" s="8"/>
-      <c r="AX8" s="8"/>
-      <c r="AY8" s="8"/>
-      <c r="AZ8" s="8"/>
-      <c r="BA8" s="8"/>
-      <c r="BB8" s="8"/>
-      <c r="BC8" s="8"/>
-      <c r="BD8" s="8"/>
-      <c r="BE8" s="8"/>
-      <c r="BF8" s="8"/>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1569,38 +1328,8 @@
       <c r="AB9" s="8">
         <v>8.6999999999999994E-3</v>
       </c>
-      <c r="AC9" s="8"/>
-      <c r="AD9" s="8"/>
-      <c r="AE9" s="8"/>
-      <c r="AF9" s="8"/>
-      <c r="AG9" s="8"/>
-      <c r="AH9" s="8"/>
-      <c r="AI9" s="8"/>
-      <c r="AJ9" s="8"/>
-      <c r="AK9" s="8"/>
-      <c r="AL9" s="8"/>
-      <c r="AM9" s="8"/>
-      <c r="AN9" s="8"/>
-      <c r="AO9" s="8"/>
-      <c r="AP9" s="8"/>
-      <c r="AQ9" s="8"/>
-      <c r="AR9" s="8"/>
-      <c r="AS9" s="8"/>
-      <c r="AT9" s="8"/>
-      <c r="AU9" s="8"/>
-      <c r="AV9" s="8"/>
-      <c r="AW9" s="8"/>
-      <c r="AX9" s="8"/>
-      <c r="AY9" s="8"/>
-      <c r="AZ9" s="8"/>
-      <c r="BA9" s="8"/>
-      <c r="BB9" s="8"/>
-      <c r="BC9" s="8"/>
-      <c r="BD9" s="8"/>
-      <c r="BE9" s="8"/>
-      <c r="BF9" s="8"/>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1685,38 +1414,8 @@
       <c r="AB10" s="8">
         <v>6.5100000000000005E-2</v>
       </c>
-      <c r="AC10" s="8"/>
-      <c r="AD10" s="8"/>
-      <c r="AE10" s="8"/>
-      <c r="AF10" s="8"/>
-      <c r="AG10" s="8"/>
-      <c r="AH10" s="8"/>
-      <c r="AI10" s="8"/>
-      <c r="AJ10" s="8"/>
-      <c r="AK10" s="8"/>
-      <c r="AL10" s="8"/>
-      <c r="AM10" s="8"/>
-      <c r="AN10" s="8"/>
-      <c r="AO10" s="8"/>
-      <c r="AP10" s="8"/>
-      <c r="AQ10" s="8"/>
-      <c r="AR10" s="8"/>
-      <c r="AS10" s="8"/>
-      <c r="AT10" s="8"/>
-      <c r="AU10" s="8"/>
-      <c r="AV10" s="8"/>
-      <c r="AW10" s="8"/>
-      <c r="AX10" s="8"/>
-      <c r="AY10" s="8"/>
-      <c r="AZ10" s="8"/>
-      <c r="BA10" s="8"/>
-      <c r="BB10" s="8"/>
-      <c r="BC10" s="8"/>
-      <c r="BD10" s="8"/>
-      <c r="BE10" s="8"/>
-      <c r="BF10" s="8"/>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1801,38 +1500,8 @@
       <c r="AB11" s="8">
         <v>2.8899999999999999E-2</v>
       </c>
-      <c r="AC11" s="8"/>
-      <c r="AD11" s="8"/>
-      <c r="AE11" s="8"/>
-      <c r="AF11" s="8"/>
-      <c r="AG11" s="8"/>
-      <c r="AH11" s="8"/>
-      <c r="AI11" s="8"/>
-      <c r="AJ11" s="8"/>
-      <c r="AK11" s="8"/>
-      <c r="AL11" s="8"/>
-      <c r="AM11" s="8"/>
-      <c r="AN11" s="8"/>
-      <c r="AO11" s="8"/>
-      <c r="AP11" s="8"/>
-      <c r="AQ11" s="8"/>
-      <c r="AR11" s="8"/>
-      <c r="AS11" s="8"/>
-      <c r="AT11" s="8"/>
-      <c r="AU11" s="8"/>
-      <c r="AV11" s="8"/>
-      <c r="AW11" s="8"/>
-      <c r="AX11" s="8"/>
-      <c r="AY11" s="8"/>
-      <c r="AZ11" s="8"/>
-      <c r="BA11" s="8"/>
-      <c r="BB11" s="8"/>
-      <c r="BC11" s="8"/>
-      <c r="BD11" s="8"/>
-      <c r="BE11" s="8"/>
-      <c r="BF11" s="8"/>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1917,38 +1586,8 @@
       <c r="AB12" s="8">
         <v>2.75E-2</v>
       </c>
-      <c r="AC12" s="8"/>
-      <c r="AD12" s="8"/>
-      <c r="AE12" s="8"/>
-      <c r="AF12" s="8"/>
-      <c r="AG12" s="8"/>
-      <c r="AH12" s="8"/>
-      <c r="AI12" s="8"/>
-      <c r="AJ12" s="8"/>
-      <c r="AK12" s="8"/>
-      <c r="AL12" s="8"/>
-      <c r="AM12" s="8"/>
-      <c r="AN12" s="8"/>
-      <c r="AO12" s="8"/>
-      <c r="AP12" s="8"/>
-      <c r="AQ12" s="8"/>
-      <c r="AR12" s="8"/>
-      <c r="AS12" s="8"/>
-      <c r="AT12" s="8"/>
-      <c r="AU12" s="8"/>
-      <c r="AV12" s="8"/>
-      <c r="AW12" s="8"/>
-      <c r="AX12" s="8"/>
-      <c r="AY12" s="8"/>
-      <c r="AZ12" s="8"/>
-      <c r="BA12" s="8"/>
-      <c r="BB12" s="8"/>
-      <c r="BC12" s="8"/>
-      <c r="BD12" s="8"/>
-      <c r="BE12" s="8"/>
-      <c r="BF12" s="8"/>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2033,38 +1672,8 @@
       <c r="AB13" s="8">
         <v>5.0200000000000002E-2</v>
       </c>
-      <c r="AC13" s="8"/>
-      <c r="AD13" s="8"/>
-      <c r="AE13" s="8"/>
-      <c r="AF13" s="8"/>
-      <c r="AG13" s="8"/>
-      <c r="AH13" s="8"/>
-      <c r="AI13" s="8"/>
-      <c r="AJ13" s="8"/>
-      <c r="AK13" s="8"/>
-      <c r="AL13" s="8"/>
-      <c r="AM13" s="8"/>
-      <c r="AN13" s="8"/>
-      <c r="AO13" s="8"/>
-      <c r="AP13" s="8"/>
-      <c r="AQ13" s="8"/>
-      <c r="AR13" s="8"/>
-      <c r="AS13" s="8"/>
-      <c r="AT13" s="8"/>
-      <c r="AU13" s="8"/>
-      <c r="AV13" s="8"/>
-      <c r="AW13" s="8"/>
-      <c r="AX13" s="8"/>
-      <c r="AY13" s="8"/>
-      <c r="AZ13" s="8"/>
-      <c r="BA13" s="8"/>
-      <c r="BB13" s="8"/>
-      <c r="BC13" s="8"/>
-      <c r="BD13" s="8"/>
-      <c r="BE13" s="8"/>
-      <c r="BF13" s="8"/>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2149,38 +1758,8 @@
       <c r="AB14" s="8">
         <v>4.7600000000000003E-2</v>
       </c>
-      <c r="AC14" s="8"/>
-      <c r="AD14" s="8"/>
-      <c r="AE14" s="8"/>
-      <c r="AF14" s="8"/>
-      <c r="AG14" s="8"/>
-      <c r="AH14" s="8"/>
-      <c r="AI14" s="8"/>
-      <c r="AJ14" s="8"/>
-      <c r="AK14" s="8"/>
-      <c r="AL14" s="8"/>
-      <c r="AM14" s="8"/>
-      <c r="AN14" s="8"/>
-      <c r="AO14" s="8"/>
-      <c r="AP14" s="8"/>
-      <c r="AQ14" s="8"/>
-      <c r="AR14" s="8"/>
-      <c r="AS14" s="8"/>
-      <c r="AT14" s="8"/>
-      <c r="AU14" s="8"/>
-      <c r="AV14" s="8"/>
-      <c r="AW14" s="8"/>
-      <c r="AX14" s="8"/>
-      <c r="AY14" s="8"/>
-      <c r="AZ14" s="8"/>
-      <c r="BA14" s="8"/>
-      <c r="BB14" s="8"/>
-      <c r="BC14" s="8"/>
-      <c r="BD14" s="8"/>
-      <c r="BE14" s="8"/>
-      <c r="BF14" s="8"/>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2265,38 +1844,8 @@
       <c r="AB15" s="8">
         <v>4.9799999999999997E-2</v>
       </c>
-      <c r="AC15" s="8"/>
-      <c r="AD15" s="8"/>
-      <c r="AE15" s="8"/>
-      <c r="AF15" s="8"/>
-      <c r="AG15" s="8"/>
-      <c r="AH15" s="8"/>
-      <c r="AI15" s="8"/>
-      <c r="AJ15" s="8"/>
-      <c r="AK15" s="8"/>
-      <c r="AL15" s="8"/>
-      <c r="AM15" s="8"/>
-      <c r="AN15" s="8"/>
-      <c r="AO15" s="8"/>
-      <c r="AP15" s="8"/>
-      <c r="AQ15" s="8"/>
-      <c r="AR15" s="8"/>
-      <c r="AS15" s="8"/>
-      <c r="AT15" s="8"/>
-      <c r="AU15" s="8"/>
-      <c r="AV15" s="8"/>
-      <c r="AW15" s="8"/>
-      <c r="AX15" s="8"/>
-      <c r="AY15" s="8"/>
-      <c r="AZ15" s="8"/>
-      <c r="BA15" s="8"/>
-      <c r="BB15" s="8"/>
-      <c r="BC15" s="8"/>
-      <c r="BD15" s="8"/>
-      <c r="BE15" s="8"/>
-      <c r="BF15" s="8"/>
     </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2381,38 +1930,8 @@
       <c r="AB16" s="8">
         <v>0.01</v>
       </c>
-      <c r="AC16" s="8"/>
-      <c r="AD16" s="8"/>
-      <c r="AE16" s="8"/>
-      <c r="AF16" s="8"/>
-      <c r="AG16" s="8"/>
-      <c r="AH16" s="8"/>
-      <c r="AI16" s="8"/>
-      <c r="AJ16" s="8"/>
-      <c r="AK16" s="8"/>
-      <c r="AL16" s="8"/>
-      <c r="AM16" s="8"/>
-      <c r="AN16" s="8"/>
-      <c r="AO16" s="8"/>
-      <c r="AP16" s="8"/>
-      <c r="AQ16" s="8"/>
-      <c r="AR16" s="8"/>
-      <c r="AS16" s="8"/>
-      <c r="AT16" s="8"/>
-      <c r="AU16" s="8"/>
-      <c r="AV16" s="8"/>
-      <c r="AW16" s="8"/>
-      <c r="AX16" s="8"/>
-      <c r="AY16" s="8"/>
-      <c r="AZ16" s="8"/>
-      <c r="BA16" s="8"/>
-      <c r="BB16" s="8"/>
-      <c r="BC16" s="8"/>
-      <c r="BD16" s="8"/>
-      <c r="BE16" s="8"/>
-      <c r="BF16" s="8"/>
     </row>
-    <row r="17" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2497,38 +2016,8 @@
       <c r="AB17" s="8">
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="AC17" s="8"/>
-      <c r="AD17" s="8"/>
-      <c r="AE17" s="8"/>
-      <c r="AF17" s="8"/>
-      <c r="AG17" s="8"/>
-      <c r="AH17" s="8"/>
-      <c r="AI17" s="8"/>
-      <c r="AJ17" s="8"/>
-      <c r="AK17" s="8"/>
-      <c r="AL17" s="8"/>
-      <c r="AM17" s="8"/>
-      <c r="AN17" s="8"/>
-      <c r="AO17" s="8"/>
-      <c r="AP17" s="8"/>
-      <c r="AQ17" s="8"/>
-      <c r="AR17" s="8"/>
-      <c r="AS17" s="8"/>
-      <c r="AT17" s="8"/>
-      <c r="AU17" s="8"/>
-      <c r="AV17" s="8"/>
-      <c r="AW17" s="8"/>
-      <c r="AX17" s="8"/>
-      <c r="AY17" s="8"/>
-      <c r="AZ17" s="8"/>
-      <c r="BA17" s="8"/>
-      <c r="BB17" s="8"/>
-      <c r="BC17" s="8"/>
-      <c r="BD17" s="8"/>
-      <c r="BE17" s="8"/>
-      <c r="BF17" s="8"/>
     </row>
-    <row r="18" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2613,38 +2102,8 @@
       <c r="AB18" s="8">
         <v>0</v>
       </c>
-      <c r="AC18" s="8"/>
-      <c r="AD18" s="8"/>
-      <c r="AE18" s="8"/>
-      <c r="AF18" s="8"/>
-      <c r="AG18" s="8"/>
-      <c r="AH18" s="8"/>
-      <c r="AI18" s="8"/>
-      <c r="AJ18" s="8"/>
-      <c r="AK18" s="8"/>
-      <c r="AL18" s="8"/>
-      <c r="AM18" s="8"/>
-      <c r="AN18" s="8"/>
-      <c r="AO18" s="8"/>
-      <c r="AP18" s="8"/>
-      <c r="AQ18" s="8"/>
-      <c r="AR18" s="8"/>
-      <c r="AS18" s="8"/>
-      <c r="AT18" s="8"/>
-      <c r="AU18" s="8"/>
-      <c r="AV18" s="8"/>
-      <c r="AW18" s="8"/>
-      <c r="AX18" s="8"/>
-      <c r="AY18" s="8"/>
-      <c r="AZ18" s="8"/>
-      <c r="BA18" s="8"/>
-      <c r="BB18" s="8"/>
-      <c r="BC18" s="8"/>
-      <c r="BD18" s="8"/>
-      <c r="BE18" s="8"/>
-      <c r="BF18" s="8"/>
     </row>
-    <row r="19" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2729,38 +2188,8 @@
       <c r="AB19" s="8">
         <v>6.6699999999999995E-2</v>
       </c>
-      <c r="AC19" s="8"/>
-      <c r="AD19" s="8"/>
-      <c r="AE19" s="8"/>
-      <c r="AF19" s="8"/>
-      <c r="AG19" s="8"/>
-      <c r="AH19" s="8"/>
-      <c r="AI19" s="8"/>
-      <c r="AJ19" s="8"/>
-      <c r="AK19" s="8"/>
-      <c r="AL19" s="8"/>
-      <c r="AM19" s="8"/>
-      <c r="AN19" s="8"/>
-      <c r="AO19" s="8"/>
-      <c r="AP19" s="8"/>
-      <c r="AQ19" s="8"/>
-      <c r="AR19" s="8"/>
-      <c r="AS19" s="8"/>
-      <c r="AT19" s="8"/>
-      <c r="AU19" s="8"/>
-      <c r="AV19" s="8"/>
-      <c r="AW19" s="8"/>
-      <c r="AX19" s="8"/>
-      <c r="AY19" s="8"/>
-      <c r="AZ19" s="8"/>
-      <c r="BA19" s="8"/>
-      <c r="BB19" s="8"/>
-      <c r="BC19" s="8"/>
-      <c r="BD19" s="8"/>
-      <c r="BE19" s="8"/>
-      <c r="BF19" s="8"/>
     </row>
-    <row r="20" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2845,38 +2274,8 @@
       <c r="AB20" s="8">
         <v>0</v>
       </c>
-      <c r="AC20" s="8"/>
-      <c r="AD20" s="8"/>
-      <c r="AE20" s="8"/>
-      <c r="AF20" s="8"/>
-      <c r="AG20" s="8"/>
-      <c r="AH20" s="8"/>
-      <c r="AI20" s="8"/>
-      <c r="AJ20" s="8"/>
-      <c r="AK20" s="8"/>
-      <c r="AL20" s="8"/>
-      <c r="AM20" s="8"/>
-      <c r="AN20" s="8"/>
-      <c r="AO20" s="8"/>
-      <c r="AP20" s="8"/>
-      <c r="AQ20" s="8"/>
-      <c r="AR20" s="8"/>
-      <c r="AS20" s="8"/>
-      <c r="AT20" s="8"/>
-      <c r="AU20" s="8"/>
-      <c r="AV20" s="8"/>
-      <c r="AW20" s="8"/>
-      <c r="AX20" s="8"/>
-      <c r="AY20" s="8"/>
-      <c r="AZ20" s="8"/>
-      <c r="BA20" s="8"/>
-      <c r="BB20" s="8"/>
-      <c r="BC20" s="8"/>
-      <c r="BD20" s="8"/>
-      <c r="BE20" s="8"/>
-      <c r="BF20" s="8"/>
     </row>
-    <row r="21" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2961,38 +2360,8 @@
       <c r="AB21" s="8">
         <v>0</v>
       </c>
-      <c r="AC21" s="8"/>
-      <c r="AD21" s="8"/>
-      <c r="AE21" s="8"/>
-      <c r="AF21" s="8"/>
-      <c r="AG21" s="8"/>
-      <c r="AH21" s="8"/>
-      <c r="AI21" s="8"/>
-      <c r="AJ21" s="8"/>
-      <c r="AK21" s="8"/>
-      <c r="AL21" s="8"/>
-      <c r="AM21" s="8"/>
-      <c r="AN21" s="8"/>
-      <c r="AO21" s="8"/>
-      <c r="AP21" s="8"/>
-      <c r="AQ21" s="8"/>
-      <c r="AR21" s="8"/>
-      <c r="AS21" s="8"/>
-      <c r="AT21" s="8"/>
-      <c r="AU21" s="8"/>
-      <c r="AV21" s="8"/>
-      <c r="AW21" s="8"/>
-      <c r="AX21" s="8"/>
-      <c r="AY21" s="8"/>
-      <c r="AZ21" s="8"/>
-      <c r="BA21" s="8"/>
-      <c r="BB21" s="8"/>
-      <c r="BC21" s="8"/>
-      <c r="BD21" s="8"/>
-      <c r="BE21" s="8"/>
-      <c r="BF21" s="8"/>
     </row>
-    <row r="22" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3077,38 +2446,8 @@
       <c r="AB22" s="8">
         <v>5.8799999999999998E-2</v>
       </c>
-      <c r="AC22" s="8"/>
-      <c r="AD22" s="8"/>
-      <c r="AE22" s="8"/>
-      <c r="AF22" s="8"/>
-      <c r="AG22" s="8"/>
-      <c r="AH22" s="8"/>
-      <c r="AI22" s="8"/>
-      <c r="AJ22" s="8"/>
-      <c r="AK22" s="8"/>
-      <c r="AL22" s="8"/>
-      <c r="AM22" s="8"/>
-      <c r="AN22" s="8"/>
-      <c r="AO22" s="8"/>
-      <c r="AP22" s="8"/>
-      <c r="AQ22" s="8"/>
-      <c r="AR22" s="8"/>
-      <c r="AS22" s="8"/>
-      <c r="AT22" s="8"/>
-      <c r="AU22" s="8"/>
-      <c r="AV22" s="8"/>
-      <c r="AW22" s="8"/>
-      <c r="AX22" s="8"/>
-      <c r="AY22" s="8"/>
-      <c r="AZ22" s="8"/>
-      <c r="BA22" s="8"/>
-      <c r="BB22" s="8"/>
-      <c r="BC22" s="8"/>
-      <c r="BD22" s="8"/>
-      <c r="BE22" s="8"/>
-      <c r="BF22" s="8"/>
     </row>
-    <row r="23" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -3193,38 +2532,8 @@
       <c r="AB23" s="8">
         <v>5.8799999999999998E-2</v>
       </c>
-      <c r="AC23" s="8"/>
-      <c r="AD23" s="8"/>
-      <c r="AE23" s="8"/>
-      <c r="AF23" s="8"/>
-      <c r="AG23" s="8"/>
-      <c r="AH23" s="8"/>
-      <c r="AI23" s="8"/>
-      <c r="AJ23" s="8"/>
-      <c r="AK23" s="8"/>
-      <c r="AL23" s="8"/>
-      <c r="AM23" s="8"/>
-      <c r="AN23" s="8"/>
-      <c r="AO23" s="8"/>
-      <c r="AP23" s="8"/>
-      <c r="AQ23" s="8"/>
-      <c r="AR23" s="8"/>
-      <c r="AS23" s="8"/>
-      <c r="AT23" s="8"/>
-      <c r="AU23" s="8"/>
-      <c r="AV23" s="8"/>
-      <c r="AW23" s="8"/>
-      <c r="AX23" s="8"/>
-      <c r="AY23" s="8"/>
-      <c r="AZ23" s="8"/>
-      <c r="BA23" s="8"/>
-      <c r="BB23" s="8"/>
-      <c r="BC23" s="8"/>
-      <c r="BD23" s="8"/>
-      <c r="BE23" s="8"/>
-      <c r="BF23" s="8"/>
     </row>
-    <row r="24" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -3309,38 +2618,8 @@
       <c r="AB24" s="8">
         <v>6.8199999999999997E-2</v>
       </c>
-      <c r="AC24" s="8"/>
-      <c r="AD24" s="8"/>
-      <c r="AE24" s="8"/>
-      <c r="AF24" s="8"/>
-      <c r="AG24" s="8"/>
-      <c r="AH24" s="8"/>
-      <c r="AI24" s="8"/>
-      <c r="AJ24" s="8"/>
-      <c r="AK24" s="8"/>
-      <c r="AL24" s="8"/>
-      <c r="AM24" s="8"/>
-      <c r="AN24" s="8"/>
-      <c r="AO24" s="8"/>
-      <c r="AP24" s="8"/>
-      <c r="AQ24" s="8"/>
-      <c r="AR24" s="8"/>
-      <c r="AS24" s="8"/>
-      <c r="AT24" s="8"/>
-      <c r="AU24" s="8"/>
-      <c r="AV24" s="8"/>
-      <c r="AW24" s="8"/>
-      <c r="AX24" s="8"/>
-      <c r="AY24" s="8"/>
-      <c r="AZ24" s="8"/>
-      <c r="BA24" s="8"/>
-      <c r="BB24" s="8"/>
-      <c r="BC24" s="8"/>
-      <c r="BD24" s="8"/>
-      <c r="BE24" s="8"/>
-      <c r="BF24" s="8"/>
     </row>
-    <row r="25" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -3425,38 +2704,8 @@
       <c r="AB25" s="8">
         <v>9.6799999999999997E-2</v>
       </c>
-      <c r="AC25" s="8"/>
-      <c r="AD25" s="8"/>
-      <c r="AE25" s="8"/>
-      <c r="AF25" s="8"/>
-      <c r="AG25" s="8"/>
-      <c r="AH25" s="8"/>
-      <c r="AI25" s="8"/>
-      <c r="AJ25" s="8"/>
-      <c r="AK25" s="8"/>
-      <c r="AL25" s="8"/>
-      <c r="AM25" s="8"/>
-      <c r="AN25" s="8"/>
-      <c r="AO25" s="8"/>
-      <c r="AP25" s="8"/>
-      <c r="AQ25" s="8"/>
-      <c r="AR25" s="8"/>
-      <c r="AS25" s="8"/>
-      <c r="AT25" s="8"/>
-      <c r="AU25" s="8"/>
-      <c r="AV25" s="8"/>
-      <c r="AW25" s="8"/>
-      <c r="AX25" s="8"/>
-      <c r="AY25" s="8"/>
-      <c r="AZ25" s="8"/>
-      <c r="BA25" s="8"/>
-      <c r="BB25" s="8"/>
-      <c r="BC25" s="8"/>
-      <c r="BD25" s="8"/>
-      <c r="BE25" s="8"/>
-      <c r="BF25" s="8"/>
     </row>
-    <row r="26" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -3541,38 +2790,8 @@
       <c r="AB26" s="8">
         <v>0.13039999999999999</v>
       </c>
-      <c r="AC26" s="8"/>
-      <c r="AD26" s="8"/>
-      <c r="AE26" s="8"/>
-      <c r="AF26" s="8"/>
-      <c r="AG26" s="8"/>
-      <c r="AH26" s="8"/>
-      <c r="AI26" s="8"/>
-      <c r="AJ26" s="8"/>
-      <c r="AK26" s="8"/>
-      <c r="AL26" s="8"/>
-      <c r="AM26" s="8"/>
-      <c r="AN26" s="8"/>
-      <c r="AO26" s="8"/>
-      <c r="AP26" s="8"/>
-      <c r="AQ26" s="8"/>
-      <c r="AR26" s="8"/>
-      <c r="AS26" s="8"/>
-      <c r="AT26" s="8"/>
-      <c r="AU26" s="8"/>
-      <c r="AV26" s="8"/>
-      <c r="AW26" s="8"/>
-      <c r="AX26" s="8"/>
-      <c r="AY26" s="8"/>
-      <c r="AZ26" s="8"/>
-      <c r="BA26" s="8"/>
-      <c r="BB26" s="8"/>
-      <c r="BC26" s="8"/>
-      <c r="BD26" s="8"/>
-      <c r="BE26" s="8"/>
-      <c r="BF26" s="8"/>
     </row>
-    <row r="27" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -3657,38 +2876,8 @@
       <c r="AB27" s="8">
         <v>6.6699999999999995E-2</v>
       </c>
-      <c r="AC27" s="8"/>
-      <c r="AD27" s="8"/>
-      <c r="AE27" s="8"/>
-      <c r="AF27" s="8"/>
-      <c r="AG27" s="8"/>
-      <c r="AH27" s="8"/>
-      <c r="AI27" s="8"/>
-      <c r="AJ27" s="8"/>
-      <c r="AK27" s="8"/>
-      <c r="AL27" s="8"/>
-      <c r="AM27" s="8"/>
-      <c r="AN27" s="8"/>
-      <c r="AO27" s="8"/>
-      <c r="AP27" s="8"/>
-      <c r="AQ27" s="8"/>
-      <c r="AR27" s="8"/>
-      <c r="AS27" s="8"/>
-      <c r="AT27" s="8"/>
-      <c r="AU27" s="8"/>
-      <c r="AV27" s="8"/>
-      <c r="AW27" s="8"/>
-      <c r="AX27" s="8"/>
-      <c r="AY27" s="8"/>
-      <c r="AZ27" s="8"/>
-      <c r="BA27" s="8"/>
-      <c r="BB27" s="8"/>
-      <c r="BC27" s="8"/>
-      <c r="BD27" s="8"/>
-      <c r="BE27" s="8"/>
-      <c r="BF27" s="8"/>
     </row>
-    <row r="28" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -3773,36 +2962,6 @@
       <c r="AB28" s="8">
         <v>8.8200000000000001E-2</v>
       </c>
-      <c r="AC28" s="8"/>
-      <c r="AD28" s="8"/>
-      <c r="AE28" s="8"/>
-      <c r="AF28" s="8"/>
-      <c r="AG28" s="8"/>
-      <c r="AH28" s="8"/>
-      <c r="AI28" s="8"/>
-      <c r="AJ28" s="8"/>
-      <c r="AK28" s="8"/>
-      <c r="AL28" s="8"/>
-      <c r="AM28" s="8"/>
-      <c r="AN28" s="8"/>
-      <c r="AO28" s="8"/>
-      <c r="AP28" s="8"/>
-      <c r="AQ28" s="8"/>
-      <c r="AR28" s="8"/>
-      <c r="AS28" s="8"/>
-      <c r="AT28" s="8"/>
-      <c r="AU28" s="8"/>
-      <c r="AV28" s="8"/>
-      <c r="AW28" s="8"/>
-      <c r="AX28" s="8"/>
-      <c r="AY28" s="8"/>
-      <c r="AZ28" s="8"/>
-      <c r="BA28" s="8"/>
-      <c r="BB28" s="8"/>
-      <c r="BC28" s="8"/>
-      <c r="BD28" s="8"/>
-      <c r="BE28" s="8"/>
-      <c r="BF28" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>